<commit_message>
fixing script automation BI fast transfer
</commit_message>
<xml_diff>
--- a/DataExcel/Transfer BI FAST.xlsx
+++ b/DataExcel/Transfer BI FAST.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nobu\main\Android-Automation\DataExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FBCC7C-8205-4BEA-A46B-88B5D744B980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7873914-19C5-4218-BC52-0C49D4CBB4DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6427804E-2AB9-E041-9637-7FB925D94670}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>Scenario</t>
   </si>
@@ -67,13 +67,13 @@
     <t>Positive</t>
   </si>
   <si>
-    <t>000000000529</t>
-  </si>
-  <si>
-    <t>Rekening No BIFAST BCA</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pin yang di masukan Salah </t>
+  </si>
+  <si>
+    <t>BankTujuan</t>
+  </si>
+  <si>
+    <t>Digital</t>
   </si>
 </sst>
 </file>
@@ -434,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BE9B16F-6A28-C24B-853E-7054B13B1283}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -446,9 +446,10 @@
     <col min="3" max="3" width="18.125" customWidth="1"/>
     <col min="4" max="4" width="32.625" customWidth="1"/>
     <col min="5" max="5" width="16.5" customWidth="1"/>
+    <col min="6" max="6" width="29.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -464,8 +465,11 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="16.5">
+    <row r="2" spans="1:6" ht="16.5">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -478,81 +482,82 @@
       <c r="D2" s="1">
         <v>1000000</v>
       </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6" ht="16.5">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
+      <c r="C3" s="2">
+        <v>510654301</v>
       </c>
       <c r="D3" s="1">
-        <v>1000000</v>
+        <v>9999</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.5">
+    <row r="4" spans="1:6" ht="16.5">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="2">
-        <v>1234567890</v>
+        <v>510654301</v>
       </c>
       <c r="D4" s="1">
-        <v>99999</v>
+        <v>250000100</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16.5">
+    <row r="5" spans="1:6" ht="16.5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="2">
-        <v>1234567890</v>
+        <v>510654301</v>
       </c>
       <c r="D5" s="1">
-        <v>250000100</v>
+        <v>1000000</v>
+      </c>
+      <c r="E5">
+        <v>444444</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16.5">
+    <row r="6" spans="1:6" ht="16.5">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2">
-        <v>1234567890</v>
+        <v>510654301</v>
       </c>
       <c r="D6" s="1">
         <v>1000000</v>
       </c>
       <c r="E6">
-        <v>444444</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="16.5">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1234567890</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1000000</v>
-      </c>
-      <c r="E7">
         <v>111111</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>